<commit_message>
Refactored Range to extend Die, removed minmium, maxmimum, and dice_count setters from Range.
</commit_message>
<xml_diff>
--- a/second_rise/Method Inheritance Mapping.xlsx
+++ b/second_rise/Method Inheritance Mapping.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="46">
   <si>
     <t>Die</t>
   </si>
@@ -139,6 +139,21 @@
   </si>
   <si>
     <t>inherit(D1000)</t>
+  </si>
+  <si>
+    <t>(minimum, maximum, dice_count)</t>
+  </si>
+  <si>
+    <t>dice_count</t>
+  </si>
+  <si>
+    <t>dice_sort</t>
+  </si>
+  <si>
+    <t>_build_total</t>
+  </si>
+  <si>
+    <t>(dice_to_exclude), None</t>
   </si>
 </sst>
 </file>
@@ -484,10 +499,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -496,7 +511,7 @@
     <col min="2" max="4" width="20.7109375" style="3" customWidth="1"/>
     <col min="5" max="5" width="32.7109375" style="3" customWidth="1"/>
     <col min="6" max="6" width="28.7109375" style="3" customWidth="1"/>
-    <col min="7" max="7" width="20.7109375" style="3" customWidth="1"/>
+    <col min="7" max="7" width="32.5703125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -541,6 +556,9 @@
       <c r="F2" s="3" t="s">
         <v>38</v>
       </c>
+      <c r="G2" s="3" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
@@ -561,6 +579,9 @@
       <c r="F3" s="3" t="s">
         <v>39</v>
       </c>
+      <c r="G3" s="3" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
@@ -581,6 +602,9 @@
       <c r="F4" s="3" t="s">
         <v>25</v>
       </c>
+      <c r="G4" s="3" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
@@ -601,6 +625,9 @@
       <c r="F5" s="3" t="s">
         <v>39</v>
       </c>
+      <c r="G5" s="3" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
@@ -621,6 +648,9 @@
       <c r="F6" s="3" t="s">
         <v>39</v>
       </c>
+      <c r="G6" s="3" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
@@ -641,6 +671,9 @@
       <c r="F7" s="3" t="s">
         <v>39</v>
       </c>
+      <c r="G7" s="3" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
@@ -661,6 +694,9 @@
       <c r="F8" s="3" t="s">
         <v>39</v>
       </c>
+      <c r="G8" s="3" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
@@ -681,6 +717,9 @@
       <c r="F9" s="3" t="s">
         <v>39</v>
       </c>
+      <c r="G9" s="3" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
@@ -701,6 +740,9 @@
       <c r="F10" s="3" t="s">
         <v>39</v>
       </c>
+      <c r="G10" s="3" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
@@ -713,13 +755,16 @@
         <v>25</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>39</v>
+        <v>25</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -741,6 +786,9 @@
       <c r="F12" s="3" t="s">
         <v>39</v>
       </c>
+      <c r="G12" s="3" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
@@ -761,6 +809,9 @@
       <c r="F13" s="3" t="s">
         <v>25</v>
       </c>
+      <c r="G13" s="3" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
@@ -781,6 +832,9 @@
       <c r="F14" s="3" t="s">
         <v>25</v>
       </c>
+      <c r="G14" s="3" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
@@ -801,6 +855,9 @@
       <c r="F15" s="3" t="s">
         <v>39</v>
       </c>
+      <c r="G15" s="3" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
@@ -821,8 +878,11 @@
       <c r="F16" s="3" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G16" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>32</v>
       </c>
@@ -841,8 +901,11 @@
       <c r="F17" s="3" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G17" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>33</v>
       </c>
@@ -861,8 +924,11 @@
       <c r="F18" s="3" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G18" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>34</v>
       </c>
@@ -880,6 +946,78 @@
       </c>
       <c r="F19" s="3" t="s">
         <v>19</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added table module.  Created primary attribute table.
</commit_message>
<xml_diff>
--- a/second_rise/Method Inheritance Mapping.xlsx
+++ b/second_rise/Method Inheritance Mapping.xlsx
@@ -4,19 +4,18 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="19155" windowHeight="11565"/>
+    <workbookView xWindow="480" yWindow="105" windowWidth="19155" windowHeight="11505"/>
   </bookViews>
   <sheets>
     <sheet name="Die" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="59">
   <si>
     <t>Die</t>
   </si>
@@ -39,7 +38,7 @@
     <t>valid</t>
   </si>
   <si>
-    <t>(sides, minimum)</t>
+    <t>()</t>
   </si>
   <si>
     <t>rolled</t>
@@ -96,9 +95,6 @@
     <t>inherit(Die)</t>
   </si>
   <si>
-    <t>(minimum)</t>
-  </si>
-  <si>
     <t>dice</t>
   </si>
   <si>
@@ -129,12 +125,6 @@
     <t>D1000</t>
   </si>
   <si>
-    <t>(minimum)-&gt;Percentile.__init__()</t>
-  </si>
-  <si>
-    <t>(minimum)-&gt;D1000.__init__()</t>
-  </si>
-  <si>
     <t>inherit(Percentile)</t>
   </si>
   <si>
@@ -154,6 +144,54 @@
   </si>
   <si>
     <t>(dice_to_exclude), None</t>
+  </si>
+  <si>
+    <t>DiceSet</t>
+  </si>
+  <si>
+    <t>modifier</t>
+  </si>
+  <si>
+    <t>modifier_operator</t>
+  </si>
+  <si>
+    <t>@property(), MOD_OPERATOR[key]</t>
+  </si>
+  <si>
+    <t>stats</t>
+  </si>
+  <si>
+    <t>To Be Implemented</t>
+  </si>
+  <si>
+    <t>@property, dict{}</t>
+  </si>
+  <si>
+    <t>(), str</t>
+  </si>
+  <si>
+    <t>inherit(DiceSet)</t>
+  </si>
+  <si>
+    <t>(modifier, modifier_operator, dice)</t>
+  </si>
+  <si>
+    <t>describe</t>
+  </si>
+  <si>
+    <t>@property(), dict{}</t>
+  </si>
+  <si>
+    <t>(sides)</t>
+  </si>
+  <si>
+    <t>()-&gt;Percentile.__init__()</t>
+  </si>
+  <si>
+    <t>()-&gt;D1000.__init__()</t>
+  </si>
+  <si>
+    <t>_calculate_stats</t>
   </si>
 </sst>
 </file>
@@ -499,24 +537,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" style="3" customWidth="1"/>
+    <col min="1" max="1" width="19.42578125" style="3" customWidth="1"/>
     <col min="2" max="4" width="20.7109375" style="3" customWidth="1"/>
     <col min="5" max="5" width="32.7109375" style="3" customWidth="1"/>
     <col min="6" max="6" width="28.7109375" style="3" customWidth="1"/>
-    <col min="7" max="7" width="32.5703125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="42.140625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="32.5703125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -528,39 +567,45 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>7</v>
+        <v>55</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>24</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>37</v>
+        <v>56</v>
       </c>
       <c r="F2" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="G2" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -574,16 +619,19 @@
         <v>17</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
@@ -594,19 +642,22 @@
         <v>25</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
@@ -620,16 +671,19 @@
         <v>18</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H5" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
@@ -643,16 +697,19 @@
         <v>18</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H6" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>9</v>
       </c>
@@ -666,16 +723,19 @@
         <v>19</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>10</v>
       </c>
@@ -689,16 +749,19 @@
         <v>20</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="G8" s="3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H8" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>11</v>
       </c>
@@ -712,62 +775,71 @@
         <v>19</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="G9" s="3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H9" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="G11" s="3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H11" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>14</v>
       </c>
@@ -781,16 +853,19 @@
         <v>22</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="G12" s="3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H12" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>15</v>
       </c>
@@ -804,16 +879,19 @@
         <v>25</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>16</v>
       </c>
@@ -827,197 +905,354 @@
         <v>25</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B15" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="E15" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G15" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D15" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="E15" s="3" t="s">
+      <c r="H15" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="F15" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F18" s="3" t="s">
+      <c r="B20" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="G18" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="G20" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
-        <v>43</v>
-      </c>
       <c r="B21" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G21" s="3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H21" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>44</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G22" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
         <v>45</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="H23" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H27" s="3" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1035,16 +1270,4 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>